<commit_message>
adding text cycle and adjusted graph margins
</commit_message>
<xml_diff>
--- a/all_noseq_noanthology.xlsx
+++ b/all_noseq_noanthology.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet3!$A$1:$E$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet3!$A$1:$E$60</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
-  <si>
-    <t>Academy Award Review of Walt Disney Cartoons</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
   <si>
     <t>Walt Disney Animation Studios</t>
   </si>
@@ -45,36 +42,12 @@
     <t>Pinocchio</t>
   </si>
   <si>
-    <t>Fantasia</t>
-  </si>
-  <si>
     <t>Dumbo</t>
   </si>
   <si>
     <t>Bambi</t>
   </si>
   <si>
-    <t>Saludos Amigos</t>
-  </si>
-  <si>
-    <t>The Three Caballeros</t>
-  </si>
-  <si>
-    <t>Make Mine Music</t>
-  </si>
-  <si>
-    <t>Song of the South</t>
-  </si>
-  <si>
-    <t>Fun and Fancy Free</t>
-  </si>
-  <si>
-    <t>Melody Time</t>
-  </si>
-  <si>
-    <t>The Adventures of Ichabod and Mr. Toad</t>
-  </si>
-  <si>
     <t>Cinderella</t>
   </si>
   <si>
@@ -159,9 +132,6 @@
     <t>Tarzan</t>
   </si>
   <si>
-    <t>Fantasia 2000</t>
-  </si>
-  <si>
     <t>Dinosaur</t>
   </si>
   <si>
@@ -253,9 +223,6 @@
   </si>
   <si>
     <t>studio</t>
-  </si>
-  <si>
-    <t>Victory Through Air Power</t>
   </si>
   <si>
     <t>mom</t>
@@ -577,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,33 +558,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>13654</v>
+        <v>13870</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -628,13 +595,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>13870</v>
+        <v>14648</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -645,10 +612,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>14648</v>
+        <v>15272</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -662,13 +629,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>14928</v>
+        <v>15566</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -679,16 +646,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>15272</v>
+        <v>18309</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -696,13 +663,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>15566</v>
+        <v>18837</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -713,10 +680,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>15577</v>
+        <v>19395</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -727,13 +694,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>15904</v>
+        <v>20262</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -744,13 +711,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>16427</v>
+        <v>21579</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -761,13 +728,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>16912</v>
+        <v>22306</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -778,47 +745,47 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>17118</v>
+        <v>23370</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>17437</v>
+        <v>24763</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>17680</v>
+        <v>25926</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -829,13 +796,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>18176</v>
+        <v>26976</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -846,50 +813,50 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>18309</v>
+        <v>28195</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>18837</v>
+        <v>28298</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>19395</v>
+        <v>29777</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -897,33 +864,33 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>20262</v>
+        <v>31252</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>21579</v>
+        <v>31595</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -931,101 +898,101 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>22306</v>
+        <v>32465</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>23370</v>
+        <v>32829</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>24763</v>
+        <v>33564</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>25926</v>
+        <v>33933</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>26976</v>
+        <v>34500</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>28195</v>
+        <v>34873</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1033,67 +1000,67 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>28298</v>
+        <v>35025</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
-        <v>29777</v>
+        <v>35237</v>
       </c>
       <c r="C28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>31252</v>
+        <v>35608</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
-        <v>31595</v>
+        <v>35965</v>
       </c>
       <c r="C30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1101,47 +1068,47 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
-        <v>32465</v>
+        <v>36124</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1">
-        <v>32829</v>
+        <v>36329</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1">
-        <v>33564</v>
+        <v>36665</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1152,13 +1119,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
-        <v>33933</v>
+        <v>36875</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1169,33 +1136,33 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1">
-        <v>34500</v>
+        <v>37057</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1">
-        <v>34873</v>
+        <v>37197</v>
       </c>
       <c r="C36" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1203,33 +1170,33 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1">
-        <v>35025</v>
+        <v>37428</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1">
-        <v>35237</v>
+        <v>37587</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1237,16 +1204,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
-        <v>35608</v>
+        <v>37771</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1254,16 +1221,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
-        <v>35965</v>
+        <v>37926</v>
       </c>
       <c r="C40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1271,13 +1238,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1">
-        <v>36124</v>
+        <v>38079</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1288,33 +1255,33 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1">
-        <v>36329</v>
+        <v>38296</v>
       </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
-        <v>36511</v>
+        <v>38660</v>
       </c>
       <c r="C43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1322,16 +1289,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1">
-        <v>36665</v>
+        <v>38877</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1339,13 +1306,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1">
-        <v>36875</v>
+        <v>39171</v>
       </c>
       <c r="C45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1356,30 +1323,30 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1">
-        <v>37057</v>
+        <v>39262</v>
       </c>
       <c r="C46" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1">
-        <v>37197</v>
+        <v>39626</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1390,16 +1357,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1">
-        <v>37428</v>
+        <v>39780</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1407,50 +1374,50 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1">
-        <v>37587</v>
+        <v>39962</v>
       </c>
       <c r="C49" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1">
-        <v>37771</v>
+        <v>40158</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1">
-        <v>37926</v>
+        <v>40506</v>
       </c>
       <c r="C51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1458,13 +1425,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1">
-        <v>38079</v>
+        <v>40739</v>
       </c>
       <c r="C52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1475,13 +1442,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1">
-        <v>38296</v>
+        <v>41082</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1492,16 +1459,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1">
-        <v>38660</v>
+        <v>41215</v>
       </c>
       <c r="C54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1509,30 +1476,30 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1">
-        <v>38877</v>
+        <v>41605</v>
       </c>
       <c r="C55" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1">
-        <v>39171</v>
+        <v>41950</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1543,47 +1510,47 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" s="1">
-        <v>39262</v>
+        <v>42174</v>
       </c>
       <c r="C57" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="1">
-        <v>39626</v>
+        <v>42333</v>
       </c>
       <c r="C58" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B59" s="1">
-        <v>39780</v>
+        <v>42433</v>
       </c>
       <c r="C59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1597,10 +1564,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="1">
-        <v>39962</v>
+        <v>42697</v>
       </c>
       <c r="C60" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -1610,197 +1577,10 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1">
-        <v>40158</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1">
-        <v>40506</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="1">
-        <v>40739</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="1">
-        <v>41082</v>
-      </c>
-      <c r="C64" t="s">
-        <v>36</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="1">
-        <v>41215</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="1">
-        <v>41605</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="1">
-        <v>41950</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" s="1">
-        <v>42174</v>
-      </c>
-      <c r="C68" t="s">
-        <v>36</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>68</v>
-      </c>
-      <c r="B69" s="1">
-        <v>42333</v>
-      </c>
-      <c r="C69" t="s">
-        <v>36</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="1">
-        <v>42433</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>69</v>
-      </c>
-      <c r="B71" s="1">
-        <v>42697</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B72" s="1"/>
+      <c r="B61" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E71"/>
+  <autoFilter ref="A1:E60"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>